<commit_message>
Updated Radio Calls for AWACS
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3igen3ggy\Desktop\Excele\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0151AA08-EFA8-49A6-BD6A-D39D695FCB0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CBE15F-FC8A-4757-8B72-9CD9D1F6DCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -298,6 +298,78 @@
   </si>
   <si>
     <t>Master Arm</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>UHF</t>
+  </si>
+  <si>
+    <t>Ready for departure</t>
+  </si>
+  <si>
+    <t>CSA1</t>
+  </si>
+  <si>
+    <t>Departure</t>
+  </si>
+  <si>
+    <t>Report Airborne</t>
+  </si>
+  <si>
+    <t>AWACS</t>
+  </si>
+  <si>
+    <t>Vector to nearest threat</t>
+  </si>
+  <si>
+    <t>CSA2</t>
+  </si>
+  <si>
+    <t>Request Picture</t>
+  </si>
+  <si>
+    <t>Declare</t>
+  </si>
+  <si>
+    <t>CSA3</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Request Unrestricted Landing</t>
+  </si>
+  <si>
+    <t>TTT6</t>
+  </si>
+  <si>
+    <t>TTTTT1</t>
+  </si>
+  <si>
+    <t>Inbound for Landing</t>
+  </si>
+  <si>
+    <t>Report on final</t>
+  </si>
+  <si>
+    <t>TT4</t>
+  </si>
+  <si>
+    <t>TT2</t>
+  </si>
+  <si>
+    <t>TT1</t>
+  </si>
+  <si>
+    <t>Takeoff</t>
+  </si>
+  <si>
+    <t>Landing</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -440,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -496,6 +568,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1793,10 +1867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C36FEA-C229-4E5E-9DFF-89862ABEE857}">
-  <dimension ref="A1:T40"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,9 +1886,10 @@
     <col min="15" max="15" width="10.28515625" customWidth="1"/>
     <col min="17" max="17" width="21.7109375" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1830,9 +1905,11 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T1" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1856,9 +1933,11 @@
       <c r="R2" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U2" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1882,9 +1961,20 @@
       <c r="R3" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T3" s="2">
+        <v>3</v>
+      </c>
+      <c r="U3" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1906,9 +1996,20 @@
       <c r="R4" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T4" s="2">
+        <v>4</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="V4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1930,9 +2031,8 @@
       <c r="R5" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1958,9 +2058,11 @@
       <c r="R6" t="s">
         <v>65</v>
       </c>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1996,9 +2098,20 @@
       <c r="R7" t="s">
         <v>67</v>
       </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T7" s="2">
+        <v>7</v>
+      </c>
+      <c r="U7" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="V7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y7" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -2026,9 +2139,20 @@
       <c r="R8" t="s">
         <v>68</v>
       </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T8" s="2">
+        <v>8</v>
+      </c>
+      <c r="U8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="V8" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y8" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2052,9 +2176,20 @@
       <c r="R9" t="s">
         <v>71</v>
       </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9" s="2">
+        <v>8</v>
+      </c>
+      <c r="U9" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="V9" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y9" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2082,7 +2217,7 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2106,9 +2241,11 @@
       <c r="R11" t="s">
         <v>75</v>
       </c>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2132,9 +2269,20 @@
       <c r="R12" t="s">
         <v>77</v>
       </c>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T12" s="2">
+        <v>6</v>
+      </c>
+      <c r="U12" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="V12" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y12" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2154,9 +2302,20 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" s="2">
+        <v>6</v>
+      </c>
+      <c r="U13" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="V13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y13" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2174,9 +2333,20 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T14" s="2">
+        <v>6</v>
+      </c>
+      <c r="U14" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="V14" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y14" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2196,7 +2366,7 @@
       <c r="P15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
-Right stick button -> Switch Paddle/Brake
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132D65DE-038E-424B-A65C-3CA74D3685C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA2E223-1C63-4A68-AB93-D6EF59DAA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2136,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="3" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" t="s">
@@ -2175,7 +2175,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="18" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" t="s">

</xml_diff>

<commit_message>
-wheel brakes -> throttle hat push, pinky to throttle thumb key
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA2E223-1C63-4A68-AB93-D6EF59DAA2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F4CC14-5BC2-438A-B1DF-167352DCC229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>Az scan</t>
-  </si>
-  <si>
-    <t>Cursor Enable</t>
-  </si>
-  <si>
-    <t>Cursor Zero</t>
-  </si>
-  <si>
-    <t>Snowplow</t>
   </si>
   <si>
     <t>TMS</t>
@@ -210,9 +201,6 @@
     <t>RDR POINT</t>
   </si>
   <si>
-    <t xml:space="preserve"> and PINKY (SHIFT)</t>
-  </si>
-  <si>
     <t>ICP Buttons</t>
   </si>
   <si>
@@ -373,6 +361,12 @@
   </si>
   <si>
     <t>Paddle Switch</t>
+  </si>
+  <si>
+    <t>Pinky (Shift)</t>
+  </si>
+  <si>
+    <t>Brakes (wheels)</t>
   </si>
 </sst>
 </file>
@@ -1579,9 +1573,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>372597</xdr:colOff>
+      <xdr:colOff>370692</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>19789</xdr:rowOff>
+      <xdr:rowOff>15979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1917,26 +1911,26 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="10" max="11" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="10" max="11" width="9.88671875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1953,15 +1947,17 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="T1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="E2" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1970,21 +1966,21 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1998,30 +1994,30 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T3" s="2">
         <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="Y3" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2038,25 +2034,25 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="T4" s="2">
         <v>4</v>
       </c>
       <c r="U4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="V4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="Y4" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2073,13 +2069,13 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2090,26 +2086,26 @@
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="U6" s="19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2122,8 +2118,8 @@
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>53</v>
+      <c r="E7" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2136,36 +2132,34 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="T7" s="2">
         <v>7</v>
       </c>
       <c r="U7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="V7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2175,29 +2169,29 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="R8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="T8" s="2">
         <v>8</v>
       </c>
       <c r="U8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Y8" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2212,29 +2206,29 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="R9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T9" s="2">
         <v>8</v>
       </c>
       <c r="U9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Y9" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2249,20 +2243,20 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="R10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2275,22 +2269,22 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="R11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="U11" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2303,31 +2297,31 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="T12" s="2">
         <v>6</v>
       </c>
       <c r="U12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Y12" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2342,7 +2336,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -2352,16 +2346,16 @@
         <v>6</v>
       </c>
       <c r="U13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="Y13" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2369,7 +2363,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H14" s="2"/>
       <c r="J14" s="1"/>
@@ -2383,16 +2377,16 @@
         <v>6</v>
       </c>
       <c r="U14" t="s">
+        <v>85</v>
+      </c>
+      <c r="V14" t="s">
         <v>89</v>
       </c>
-      <c r="V14" t="s">
-        <v>93</v>
-      </c>
       <c r="Y14" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2412,7 +2406,7 @@
       <c r="P15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2429,25 +2423,25 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -2458,14 +2452,14 @@
       <c r="P17" s="7"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>7</v>
@@ -2474,27 +2468,27 @@
         <v>11</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2506,23 +2500,23 @@
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="12"/>
       <c r="O19" s="13"/>
       <c r="P19" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2542,7 +2536,7 @@
       <c r="P20" s="2"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2560,7 +2554,7 @@
       <c r="P21" s="2"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2578,7 +2572,7 @@
       <c r="P22" s="14"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2590,27 +2584,27 @@
       </c>
       <c r="H23" s="2"/>
       <c r="J23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="L23" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2622,23 +2616,23 @@
       </c>
       <c r="H24" s="2"/>
       <c r="J24" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="10"/>
       <c r="O24" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P24" s="3"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2656,7 +2650,7 @@
       <c r="P25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2678,7 +2672,7 @@
       <c r="P26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2700,7 +2694,7 @@
       <c r="P27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2718,7 +2712,7 @@
       <c r="P28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2736,7 +2730,7 @@
       <c r="P29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2756,7 +2750,7 @@
       <c r="P30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2776,7 +2770,7 @@
       <c r="P31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2794,7 +2788,7 @@
       <c r="P32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2807,14 +2801,14 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2834,7 +2828,7 @@
       <c r="P34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2847,14 +2841,14 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2872,7 +2866,7 @@
       <c r="P36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2892,7 +2886,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2900,7 +2894,7 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="H38" s="1"/>
       <c r="K38" s="1"/>
@@ -2914,16 +2908,14 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2936,16 +2928,14 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="G40" s="5"/>
       <c r="H40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>

</xml_diff>

<commit_message>
-Gremlin (added Radar hat button to modA), -Added Cursor Enable(A)/Zero(B) to Radar hat button, and Radar Freeze(A)/Snowplow(B) to throttle thumb button
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F4CC14-5BC2-438A-B1DF-167352DCC229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCA793C-3C06-45E1-8F9E-F5AB2A840056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
+    <workbookView xWindow="31215" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -368,12 +368,24 @@
   <si>
     <t>Brakes (wheels)</t>
   </si>
+  <si>
+    <t>Cursor Enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radar Freeze </t>
+  </si>
+  <si>
+    <t>Radar Snowplow</t>
+  </si>
+  <si>
+    <t>Cursor Zero</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,14 +438,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -509,7 +513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -561,9 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1910,27 +1911,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C36FEA-C229-4E5E-9DFF-89862ABEE857}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="10" max="11" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.85546875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" customWidth="1"/>
-    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1950,7 +1951,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1976,11 +1977,11 @@
       <c r="R2" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="U2" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2013,11 +2014,11 @@
       <c r="V3" t="s">
         <v>81</v>
       </c>
-      <c r="Y3" s="19" t="s">
+      <c r="Y3" s="18" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2048,11 +2049,11 @@
       <c r="V4" t="s">
         <v>84</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="Y4" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2075,7 +2076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2101,11 +2102,11 @@
       <c r="R6" t="s">
         <v>60</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="U6" s="18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -2150,16 +2151,18 @@
       <c r="V7" t="s">
         <v>92</v>
       </c>
-      <c r="Y7" s="19" t="s">
+      <c r="Y7" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2168,7 +2171,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="18" t="s">
+      <c r="O8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="P8" s="1"/>
@@ -2187,16 +2190,18 @@
       <c r="V8" t="s">
         <v>93</v>
       </c>
-      <c r="Y8" s="19" t="s">
+      <c r="Y8" s="18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2224,11 +2229,11 @@
       <c r="V9" t="s">
         <v>94</v>
       </c>
-      <c r="Y9" s="19" t="s">
+      <c r="Y9" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2256,7 +2261,7 @@
       </c>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2280,11 +2285,11 @@
       <c r="R11" t="s">
         <v>70</v>
       </c>
-      <c r="U11" s="19" t="s">
+      <c r="U11" s="18" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2317,11 +2322,11 @@
       <c r="V12" t="s">
         <v>86</v>
       </c>
-      <c r="Y12" s="19" t="s">
+      <c r="Y12" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2341,7 +2346,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-      <c r="R13" s="20"/>
+      <c r="R13" s="19"/>
       <c r="T13" s="2">
         <v>6</v>
       </c>
@@ -2351,11 +2356,11 @@
       <c r="V13" t="s">
         <v>88</v>
       </c>
-      <c r="Y13" s="19" t="s">
+      <c r="Y13" s="18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2382,11 +2387,11 @@
       <c r="V14" t="s">
         <v>89</v>
       </c>
-      <c r="Y14" s="19" t="s">
+      <c r="Y14" s="18" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2406,7 +2411,7 @@
       <c r="P15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2430,7 +2435,7 @@
       <c r="P16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2452,7 +2457,7 @@
       <c r="P17" s="7"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2488,7 +2493,7 @@
       </c>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2516,7 +2521,7 @@
       </c>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2536,7 +2541,7 @@
       <c r="P20" s="2"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2554,7 +2559,7 @@
       <c r="P21" s="2"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2572,7 +2577,7 @@
       <c r="P22" s="14"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2604,7 +2609,7 @@
       </c>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2632,7 +2637,7 @@
       <c r="P24" s="3"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2650,7 +2655,7 @@
       <c r="P25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2672,7 +2677,7 @@
       <c r="P26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2694,7 +2699,7 @@
       <c r="P27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2712,7 +2717,7 @@
       <c r="P28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2730,7 +2735,7 @@
       <c r="P29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2750,7 +2755,7 @@
       <c r="P30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2770,7 +2775,7 @@
       <c r="P31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2788,7 +2793,7 @@
       <c r="P32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2808,7 +2813,7 @@
       <c r="P33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2828,7 +2833,7 @@
       <c r="P34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2848,7 +2853,7 @@
       <c r="P35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2866,7 +2871,7 @@
       <c r="P36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2886,7 +2891,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2908,14 +2913,16 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2928,14 +2935,16 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="5"/>
+      <c r="G40" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>

</xml_diff>

<commit_message>
updated NVG and sunglasses to be on throttle
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7104FF84-CF82-429B-B5E2-8281DCB00EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5996FE9-49D2-4833-9131-DF5FC1DDD44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Cursor Zero</t>
+  </si>
+  <si>
+    <t>NightVision</t>
+  </si>
+  <si>
+    <t>Sunglasses</t>
   </si>
 </sst>
 </file>
@@ -510,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -565,6 +571,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1908,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C36FEA-C229-4E5E-9DFF-89862ABEE857}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2157,8 +2169,8 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3" t="s">
-        <v>106</v>
+      <c r="E8" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2169,7 +2181,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="5" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" t="s">
@@ -2196,9 +2208,6 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2327,7 +2336,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5" t="s">
@@ -2361,7 +2370,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
       <c r="G14" s="6" t="s">
@@ -2392,7 +2401,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
@@ -2480,10 +2489,10 @@
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O18" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>42</v>
@@ -2511,8 +2520,12 @@
         <v>76</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="13"/>
+      <c r="N19" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>41</v>
+      </c>
       <c r="P19" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
-updated NVG and sunglasses
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5996FE9-49D2-4833-9131-DF5FC1DDD44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A8F970-772B-465B-A202-1930F7ECE444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -369,19 +369,19 @@
     <t>Cursor Enable</t>
   </si>
   <si>
-    <t xml:space="preserve">Radar Freeze </t>
-  </si>
-  <si>
     <t>Radar Snowplow</t>
   </si>
   <si>
     <t>Cursor Zero</t>
   </si>
   <si>
-    <t>NightVision</t>
-  </si>
-  <si>
     <t>Sunglasses</t>
+  </si>
+  <si>
+    <t>Nightvision</t>
+  </si>
+  <si>
+    <t>Radar Freeze</t>
   </si>
 </sst>
 </file>
@@ -1920,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C36FEA-C229-4E5E-9DFF-89862ABEE857}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2170,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="21" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>41</v>
@@ -2931,7 +2931,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H39" s="1"/>
       <c r="K39" s="1"/>
@@ -2953,7 +2953,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H40" s="1"/>
       <c r="K40" s="1"/>

</xml_diff>

<commit_message>
-update radar CURSOR ENABLE added RF Switch
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2A6F39-1E89-40CB-BB28-943F3403ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C580E8F-4DDF-4B6B-A1C9-6A19F8661F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>Radar Freeze</t>
+  </si>
+  <si>
+    <t>RF Switch</t>
   </si>
 </sst>
 </file>
@@ -516,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -576,6 +579,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1921,7 +1933,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" activeCellId="1" sqref="L9 J12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2141,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2182,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -2244,7 +2256,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
@@ -2272,7 +2284,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -2489,7 +2501,7 @@
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="8" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>40</v>
@@ -2521,7 +2533,7 @@
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>41</v>
@@ -2546,7 +2558,9 @@
       <c r="K20" s="13"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="12"/>
+      <c r="N20" s="22" t="s">
+        <v>107</v>
+      </c>
       <c r="O20" s="13"/>
       <c r="P20" s="2"/>
       <c r="T20" s="1"/>
@@ -2572,7 +2586,7 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
@@ -2590,7 +2604,7 @@
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>

</xml_diff>

<commit_message>
-CMS <-> DMS swap
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C580E8F-4DDF-4B6B-A1C9-6A19F8661F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E9CDB6-6034-4873-8F96-6A3FBB313E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -581,12 +581,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1933,7 +1927,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2286,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -2320,7 +2314,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2586,7 +2580,7 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="23"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
@@ -2604,7 +2598,7 @@
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="24"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>

</xml_diff>

<commit_message>
-slap switch <-> pickle swap
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A9378A-8C36-44D4-B2CB-2DFB35393131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE5252F-D207-4449-B4D9-DE6657CFAD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1930,7 +1930,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2105,7 @@
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -2443,7 +2443,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>

</xml_diff>

<commit_message>
-Added comms switch on throttle
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C8C44E-9A8D-4422-B907-26D1CD7963FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF59C60-A7DE-4930-9573-470B6024BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>Gauges</t>
+  </si>
+  <si>
+    <t>Comms</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1930,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2284,9 @@
       <c r="E11" s="21"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>

</xml_diff>

<commit_message>
-After Mexico update - Cursor enable and zero swap
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA7B2AB-74BF-489A-A44F-B66A28441ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF9EDC-4B4B-4250-9AA1-CD96F0DEC339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="315" windowWidth="21600" windowHeight="11385" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -1942,7 +1942,7 @@
   <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -2191,7 +2191,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>

</xml_diff>

<commit_message>
next AG weapon added
</commit_message>
<xml_diff>
--- a/3igen3ggy helpers/Joystick mappings.xlsx
+++ b/3igen3ggy helpers/Joystick mappings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Falcon BMS 4.37\User\Config\3igen3ggy helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF9EDC-4B4B-4250-9AA1-CD96F0DEC339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F296EE7-1720-4577-B26A-9A3033715C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="315" windowWidth="21600" windowHeight="11385" xr2:uid="{09266651-1A48-4D99-85F2-9CD934D8CEA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="119">
   <si>
     <t>Anetnna elevation</t>
   </si>
@@ -401,12 +401,15 @@
   <si>
     <t>F11</t>
   </si>
+  <si>
+    <t>AG Next Weapon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +462,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -534,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -596,6 +607,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1941,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C36FEA-C229-4E5E-9DFF-89862ABEE857}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,7 +2842,9 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="23" t="s">
+        <v>118</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>

</xml_diff>